<commit_message>
Updated to new project name (PS_Fgen_HW), removed Z-Diode and ATX_PWR_ON signal from MainBoard
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/CAMOutputs/Assembly/MainBoard_PartsList.xlsx
+++ b/Electrical/MainBoard/CAMOutputs/Assembly/MainBoard_PartsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\V17\Dokumente\EAGLE\projects\PowerSupplySigGen\MainBoard\v1.2\CAMOutputs\Assembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\V17\Dokumente\EAGLE\projects\PS_Fgen_HW\Electrical\MainBoard\CAMOutputs\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{450BBCFA-D3B0-4121-8310-1D81D934D979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E68181-3663-4A7C-896D-8A8E1D830E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBoard" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="119">
   <si>
     <t>Qty</t>
   </si>
@@ -374,12 +374,15 @@
   </si>
   <si>
     <t>R24, R43, R44, R45, R46</t>
+  </si>
+  <si>
+    <t>MEGA1284-P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1437,11 +1440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2094,7 @@
         <v>102</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
MainBoard: Removed ATX_5V_SB input (combined VCC and +5V nets)
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/CAMOutputs/Assembly/MainBoard_PartsList.xlsx
+++ b/Electrical/MainBoard/CAMOutputs/Assembly/MainBoard_PartsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\V17\Dokumente\EAGLE\projects\PS_Fgen_HW\Electrical\MainBoard\CAMOutputs\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E68181-3663-4A7C-896D-8A8E1D830E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58D08F1-313F-4C19-BA78-26E662A2F646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>2,54/1,0</t>
   </si>
   <si>
-    <t>+3V3_OUT, +5V_OUT, +12V_OUT, -12V_OUT, ATX_+3V3, ATX_+5V, ATX_+5V_SB, ATX_+12V, ATX_-12V, ATX_GND, ATX_PWRON, DVM1, DVM2, GND_1, GND_2, GND_3, GND_4, GND_DVM, GND_OUT1, GND_OUT2, GND_OUT3, OUT1, OUT2, OUT3</t>
-  </si>
-  <si>
     <t>THROUGH-HOLE PAD</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>MEGA1284-P</t>
+  </si>
+  <si>
+    <t>+3V3_OUT, +5V_OUT, +12V_OUT, -12V_OUT, ATX_+3V3, ATX_+5V, ATX_+12V, ATX_-12V, ATX_GND, DVM1, DVM2, GND_1, GND_2, GND_3, GND_4, GND_DVM, GND_OUT1, GND_OUT2, GND_OUT3, OUT1, OUT2, OUT3</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1085,6 +1085,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1443,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1462,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1486,17 +1489,17 @@
     </row>
     <row r="4" spans="1:5" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1505,13 +1508,13 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,13 +1523,13 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,13 +1538,13 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1550,13 +1553,13 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,16 +1567,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1581,16 +1584,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,16 +1601,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1615,16 +1618,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,16 +1635,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1649,16 +1652,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1683,16 +1686,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1700,16 +1703,16 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,16 +1720,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1734,16 +1737,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,16 +1754,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1768,16 +1771,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,16 +1788,16 @@
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,16 +1805,16 @@
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,16 +1822,16 @@
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E24" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,16 +1839,16 @@
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E25" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1853,16 +1856,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E26" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,16 +1873,16 @@
         <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E27" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1887,16 +1890,16 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,16 +1907,16 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1921,16 +1924,16 @@
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1955,16 +1958,16 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E32" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,16 +1975,16 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1989,16 +1992,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2006,16 +2009,16 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2023,16 +2026,16 @@
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2040,16 +2043,16 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2057,16 +2060,16 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,16 +2077,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2091,16 +2094,16 @@
         <v>1</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2108,16 +2111,16 @@
         <v>1</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2125,16 +2128,16 @@
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E42" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2142,16 +2145,16 @@
         <v>2</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="9" t="s">
+      <c r="E43" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>